<commit_message>
ajuste de carga masiva
</commit_message>
<xml_diff>
--- a/front/src/storage/usuarios.xlsx
+++ b/front/src/storage/usuarios.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Plantilla carga masiva de usuarios</t>
   </si>
@@ -97,9 +97,6 @@
     <t>foto</t>
   </si>
   <si>
-    <t>jesus andres</t>
-  </si>
-  <si>
     <t>almeda perez</t>
   </si>
   <si>
@@ -143,13 +140,34 @@
   </si>
   <si>
     <t>visitante</t>
+  </si>
+  <si>
+    <t>jesus 1</t>
+  </si>
+  <si>
+    <t>jesus 2</t>
+  </si>
+  <si>
+    <t>jesus 3</t>
+  </si>
+  <si>
+    <t>jesus 4</t>
+  </si>
+  <si>
+    <t>jesus 5</t>
+  </si>
+  <si>
+    <t>jesus 6</t>
+  </si>
+  <si>
+    <t>jesus 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,14 +197,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -266,7 +276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,9 +290,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -564,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="A2:J2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -584,18 +591,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -643,22 +650,22 @@
         <v>25859444</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -675,22 +682,22 @@
         <v>25859565</v>
       </c>
       <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -704,25 +711,25 @@
         <v>5054</v>
       </c>
       <c r="D5">
-        <v>25859444</v>
+        <v>25859521</v>
       </c>
       <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -736,25 +743,25 @@
         <v>5055</v>
       </c>
       <c r="D6">
-        <v>25859444</v>
+        <v>25152132</v>
       </c>
       <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -765,28 +772,28 @@
         <v>151</v>
       </c>
       <c r="C7">
-        <v>5555</v>
+        <v>1551</v>
       </c>
       <c r="D7">
-        <v>25859444</v>
+        <v>15151451</v>
       </c>
       <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -800,25 +807,25 @@
         <v>5555</v>
       </c>
       <c r="D8">
-        <v>25859444</v>
+        <v>15484515</v>
       </c>
       <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -826,144 +833,21 @@
         <v>25859444</v>
       </c>
       <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="E29" s="5"/>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>